<commit_message>
hopeful simple fix overlook
</commit_message>
<xml_diff>
--- a/out/production/Algorithms_Assignment_1/testfiles/Comparison.xlsx
+++ b/out/production/Algorithms_Assignment_1/testfiles/Comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Algorithms_Assignment_1\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027C104C-342F-4956-96DA-A6C113090F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6954B400-8D3E-4CB6-A5C9-8E02628C2959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Map size</t>
   </si>
@@ -36,9 +36,6 @@
     <t>BFS solution steps</t>
   </si>
   <si>
-    <t>DFS actual stesp</t>
-  </si>
-  <si>
     <t>BFS actual steps</t>
   </si>
   <si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t>Maze100_4.txt</t>
+  </si>
+  <si>
+    <t>34ms</t>
+  </si>
+  <si>
+    <t>DFS actual steps</t>
+  </si>
+  <si>
+    <t>32ms</t>
+  </si>
+  <si>
+    <t>35ms</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,136 +460,190 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>92</v>
+      </c>
+      <c r="E2">
+        <v>294</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>240</v>
+      </c>
+      <c r="E4">
+        <v>331</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>185</v>
+      </c>
+      <c r="E5">
+        <v>348</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>118</v>
+      </c>
+      <c r="E6">
+        <v>390</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>447</v>
+      </c>
+      <c r="E7">
+        <v>780</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed jar and xml files and manifest stuff
</commit_message>
<xml_diff>
--- a/out/production/Algorithms_Assignment_1/testfiles/Comparison.xlsx
+++ b/out/production/Algorithms_Assignment_1/testfiles/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Algorithms_Assignment_1\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76C1F7D-947A-4726-BF57-1508B18F4161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED53BC-03FD-4C52-B570-16A502C35CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>92</v>
@@ -560,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -586,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C4">
         <v>240</v>
@@ -638,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6">
         <v>118</v>
@@ -664,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C7">
         <v>447</v>
@@ -690,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>53</v>
@@ -716,7 +716,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9">
         <v>148</v>
@@ -742,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C10">
         <v>541</v>
@@ -794,7 +794,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12">
         <v>153</v>
@@ -872,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C15">
         <v>223</v>

</xml_diff>